<commit_message>
Remove 'pulsa_samsung' field from BastRecordModel and update related forms and exports
</commit_message>
<xml_diff>
--- a/bast/static/bast/BAST.xlsx
+++ b/bast/static/bast/BAST.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="90">
   <si>
     <t xml:space="preserve">BERITA ACARA SERAH TERIMA PUSAT GEMPA NASIONAL  </t>
   </si>
@@ -258,6 +258,9 @@
   </si>
   <si>
     <t>dilakukan dalam</t>
+  </si>
+  <si>
+    <t>Pasca bayar</t>
   </si>
   <si>
     <t>mengatasi</t>
@@ -2456,8 +2459,8 @@
   </sheetPr>
   <dimension ref="A1:X976"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="70" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55:E55"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="70" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4259259259259" defaultRowHeight="15" customHeight="1"/>
@@ -3432,8 +3435,8 @@
         <v>88154</v>
       </c>
       <c r="F37" s="85"/>
-      <c r="G37" s="84">
-        <v>0</v>
+      <c r="G37" s="84" t="s">
+        <v>77</v>
       </c>
       <c r="H37" s="85"/>
       <c r="I37" s="188"/>
@@ -3450,11 +3453,11 @@
       <c r="A38" s="1"/>
       <c r="B38" s="6"/>
       <c r="C38" s="79" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D38" s="80"/>
       <c r="E38" s="81" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F38" s="82"/>
       <c r="G38" s="82"/>
@@ -3473,7 +3476,7 @@
       <c r="A39" s="1"/>
       <c r="B39" s="6"/>
       <c r="C39" s="79" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D39" s="80"/>
       <c r="E39" s="86">
@@ -3481,7 +3484,7 @@
       </c>
       <c r="F39" s="87"/>
       <c r="G39" s="88" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H39" s="89"/>
       <c r="I39" s="188"/>
@@ -3500,11 +3503,11 @@
       <c r="C40" s="76"/>
       <c r="D40" s="90"/>
       <c r="E40" s="88" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F40" s="89"/>
       <c r="G40" s="88" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H40" s="89"/>
       <c r="I40" s="188"/>
@@ -3540,7 +3543,7 @@
       <c r="A42" s="1"/>
       <c r="B42" s="3"/>
       <c r="C42" s="30" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D42" s="93"/>
       <c r="E42" s="94"/>
@@ -3618,7 +3621,7 @@
       <c r="A46" s="1"/>
       <c r="B46" s="6"/>
       <c r="C46" s="98" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D46" s="98"/>
       <c r="E46" s="98"/>
@@ -3658,20 +3661,20 @@
       <c r="A48" s="1"/>
       <c r="B48" s="6"/>
       <c r="C48" s="101" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D48" s="102"/>
       <c r="E48" s="103"/>
       <c r="F48" s="54"/>
       <c r="G48" s="104" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H48" s="105"/>
       <c r="I48" s="199"/>
       <c r="J48" s="54"/>
       <c r="K48" s="200"/>
       <c r="L48" s="104" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="M48" s="105"/>
       <c r="N48" s="105"/>
@@ -3683,7 +3686,7 @@
       <c r="A49" s="1"/>
       <c r="B49" s="6"/>
       <c r="C49" s="106" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D49" s="107"/>
       <c r="E49" s="108"/>
@@ -3799,20 +3802,20 @@
       <c r="A55" s="1"/>
       <c r="B55" s="6"/>
       <c r="C55" s="128" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D55" s="129"/>
       <c r="E55" s="130"/>
       <c r="F55" s="54"/>
       <c r="G55" s="131" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H55" s="132"/>
       <c r="I55" s="211"/>
       <c r="J55" s="54"/>
       <c r="K55" s="200"/>
       <c r="L55" s="131" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="M55" s="132"/>
       <c r="N55" s="132"/>

</xml_diff>

<commit_message>
Add "orang" to BAST.xlsx
</commit_message>
<xml_diff>
--- a/bast/static/bast/BAST.xlsx
+++ b/bast/static/bast/BAST.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="91">
   <si>
     <t xml:space="preserve">BERITA ACARA SERAH TERIMA PUSAT GEMPA NASIONAL  </t>
   </si>
@@ -143,7 +143,10 @@
     <t>Trismahargyono</t>
   </si>
   <si>
-    <t xml:space="preserve">Jumlah Petugas Yang Hadir </t>
+    <t>Jumlah Petugas Yang Hadir</t>
+  </si>
+  <si>
+    <t>orang</t>
   </si>
   <si>
     <t>A. Tentang Gempa Bumi yang terjadi pada saat tugas shift</t>
@@ -1381,7 +1384,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="217">
+  <cellXfs count="218">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1829,6 +1832,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2459,8 +2465,8 @@
   </sheetPr>
   <dimension ref="A1:X976"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="70" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4259259259259" defaultRowHeight="15" customHeight="1"/>
@@ -2520,7 +2526,7 @@
       <c r="N2" s="5"/>
       <c r="O2" s="5"/>
       <c r="P2" s="5"/>
-      <c r="Q2" s="213"/>
+      <c r="Q2" s="214"/>
     </row>
     <row r="3" ht="18" customHeight="1" spans="1:17">
       <c r="A3" s="1"/>
@@ -2545,7 +2551,7 @@
       <c r="N3" s="141"/>
       <c r="O3" s="141"/>
       <c r="P3" s="142"/>
-      <c r="Q3" s="214"/>
+      <c r="Q3" s="215"/>
     </row>
     <row r="4" ht="18" customHeight="1" spans="1:17">
       <c r="A4" s="1"/>
@@ -2565,7 +2571,7 @@
       </c>
       <c r="O4" s="146"/>
       <c r="P4" s="147"/>
-      <c r="Q4" s="214"/>
+      <c r="Q4" s="215"/>
     </row>
     <row r="5" ht="18" customHeight="1" spans="1:17">
       <c r="A5" s="1"/>
@@ -2585,7 +2591,7 @@
       </c>
       <c r="O5" s="148"/>
       <c r="P5" s="147"/>
-      <c r="Q5" s="214"/>
+      <c r="Q5" s="215"/>
     </row>
     <row r="6" ht="18" customHeight="1" spans="1:17">
       <c r="A6" s="1"/>
@@ -2610,7 +2616,7 @@
       </c>
       <c r="O6" s="151"/>
       <c r="P6" s="152"/>
-      <c r="Q6" s="214"/>
+      <c r="Q6" s="215"/>
     </row>
     <row r="7" ht="14.4" spans="1:17">
       <c r="A7" s="1"/>
@@ -2629,7 +2635,7 @@
       <c r="N7" s="28"/>
       <c r="O7" s="28"/>
       <c r="P7" s="28"/>
-      <c r="Q7" s="214"/>
+      <c r="Q7" s="215"/>
     </row>
     <row r="8" ht="17.4" spans="1:17">
       <c r="A8" s="1"/>
@@ -2660,7 +2666,7 @@
       <c r="N8" s="145"/>
       <c r="O8" s="145"/>
       <c r="P8" s="28"/>
-      <c r="Q8" s="214"/>
+      <c r="Q8" s="215"/>
     </row>
     <row r="9" ht="17.4" spans="1:17">
       <c r="A9" s="1"/>
@@ -2691,7 +2697,7 @@
       <c r="N9" s="14"/>
       <c r="O9" s="15"/>
       <c r="P9" s="28"/>
-      <c r="Q9" s="214"/>
+      <c r="Q9" s="215"/>
     </row>
     <row r="10" ht="17.4" spans="1:17">
       <c r="A10" s="1"/>
@@ -2722,7 +2728,7 @@
       <c r="N10" s="14"/>
       <c r="O10" s="15"/>
       <c r="P10" s="28"/>
-      <c r="Q10" s="214"/>
+      <c r="Q10" s="215"/>
     </row>
     <row r="11" ht="17.4" spans="1:17">
       <c r="A11" s="1"/>
@@ -2753,7 +2759,7 @@
       <c r="N11" s="14"/>
       <c r="O11" s="15"/>
       <c r="P11" s="28"/>
-      <c r="Q11" s="214"/>
+      <c r="Q11" s="215"/>
     </row>
     <row r="12" ht="17.4" spans="1:17">
       <c r="A12" s="1"/>
@@ -2784,7 +2790,7 @@
       <c r="N12" s="14"/>
       <c r="O12" s="15"/>
       <c r="P12" s="28"/>
-      <c r="Q12" s="214"/>
+      <c r="Q12" s="215"/>
     </row>
     <row r="13" ht="17.4" spans="1:17">
       <c r="A13" s="1"/>
@@ -2815,7 +2821,7 @@
       <c r="N13" s="14"/>
       <c r="O13" s="15"/>
       <c r="P13" s="28"/>
-      <c r="Q13" s="214"/>
+      <c r="Q13" s="215"/>
     </row>
     <row r="14" ht="17.4" spans="1:17">
       <c r="A14" s="1"/>
@@ -2846,7 +2852,7 @@
       <c r="N14" s="14"/>
       <c r="O14" s="15"/>
       <c r="P14" s="28"/>
-      <c r="Q14" s="214"/>
+      <c r="Q14" s="215"/>
     </row>
     <row r="15" ht="17.4" spans="1:17">
       <c r="A15" s="1"/>
@@ -2877,7 +2883,7 @@
       <c r="N15" s="14"/>
       <c r="O15" s="15"/>
       <c r="P15" s="1"/>
-      <c r="Q15" s="214"/>
+      <c r="Q15" s="215"/>
     </row>
     <row r="16" ht="17.4" spans="1:17">
       <c r="A16" s="1"/>
@@ -2908,7 +2914,7 @@
       <c r="N16" s="14"/>
       <c r="O16" s="15"/>
       <c r="P16" s="1"/>
-      <c r="Q16" s="214"/>
+      <c r="Q16" s="215"/>
     </row>
     <row r="17" ht="15.6" spans="1:17">
       <c r="A17" s="1"/>
@@ -2939,7 +2945,7 @@
       <c r="N17" s="14"/>
       <c r="O17" s="15"/>
       <c r="P17" s="1"/>
-      <c r="Q17" s="214"/>
+      <c r="Q17" s="215"/>
     </row>
     <row r="18" ht="15.6" spans="1:17">
       <c r="A18" s="1"/>
@@ -2955,16 +2961,18 @@
         <v>38</v>
       </c>
       <c r="K18" s="51"/>
-      <c r="L18" s="19">
+      <c r="L18" s="164">
         <v>9</v>
       </c>
-      <c r="M18" s="164"/>
-      <c r="N18" s="164"/>
-      <c r="O18" s="165"/>
+      <c r="M18" s="165" t="s">
+        <v>39</v>
+      </c>
+      <c r="N18" s="165"/>
+      <c r="O18" s="166"/>
       <c r="P18" s="1"/>
-      <c r="Q18" s="214"/>
-    </row>
-    <row r="19" ht="15.15" spans="1:17">
+      <c r="Q18" s="215"/>
+    </row>
+    <row r="19" spans="1:17">
       <c r="A19" s="1"/>
       <c r="B19" s="6"/>
       <c r="C19" s="2"/>
@@ -2981,118 +2989,118 @@
       <c r="N19" s="1"/>
       <c r="O19" s="1"/>
       <c r="P19" s="1"/>
-      <c r="Q19" s="214"/>
+      <c r="Q19" s="215"/>
     </row>
     <row r="20" ht="21" spans="1:17">
       <c r="A20" s="28"/>
       <c r="B20" s="29"/>
       <c r="C20" s="30" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D20" s="31"/>
       <c r="E20" s="32"/>
       <c r="F20" s="32"/>
       <c r="G20" s="32"/>
       <c r="H20" s="32"/>
-      <c r="I20" s="166"/>
+      <c r="I20" s="167"/>
       <c r="J20" s="32"/>
-      <c r="K20" s="167"/>
+      <c r="K20" s="168"/>
       <c r="L20" s="31"/>
-      <c r="M20" s="168"/>
-      <c r="N20" s="168"/>
-      <c r="O20" s="168"/>
-      <c r="P20" s="168"/>
-      <c r="Q20" s="213"/>
+      <c r="M20" s="169"/>
+      <c r="N20" s="169"/>
+      <c r="O20" s="169"/>
+      <c r="P20" s="169"/>
+      <c r="Q20" s="214"/>
     </row>
     <row r="21" ht="15.75" customHeight="1" spans="1:17">
       <c r="A21" s="28"/>
       <c r="B21" s="33"/>
       <c r="C21" s="34" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D21" s="34"/>
       <c r="E21" s="35"/>
       <c r="F21" s="35" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G21" s="36">
         <v>7</v>
       </c>
       <c r="H21" s="35" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I21" s="154"/>
-      <c r="J21" s="169" t="s">
-        <v>43</v>
+      <c r="J21" s="170" t="s">
+        <v>44</v>
       </c>
-      <c r="K21" s="169"/>
-      <c r="L21" s="169" t="s">
-        <v>41</v>
+      <c r="K21" s="170"/>
+      <c r="L21" s="170" t="s">
+        <v>42</v>
       </c>
       <c r="M21" s="35"/>
       <c r="N21" s="34"/>
       <c r="O21" s="28"/>
       <c r="P21" s="28"/>
-      <c r="Q21" s="214"/>
+      <c r="Q21" s="215"/>
     </row>
     <row r="22" ht="15.75" customHeight="1" spans="1:17">
       <c r="A22" s="28"/>
       <c r="B22" s="33"/>
       <c r="C22" s="37" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D22" s="37"/>
       <c r="E22" s="38"/>
       <c r="F22" s="38" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G22" s="39">
         <v>4</v>
       </c>
       <c r="H22" s="38" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I22" s="154"/>
-      <c r="J22" s="217" t="s">
-        <v>45</v>
+      <c r="J22" s="218" t="s">
+        <v>46</v>
       </c>
-      <c r="K22" s="169"/>
-      <c r="L22" s="169" t="s">
-        <v>41</v>
+      <c r="K22" s="170"/>
+      <c r="L22" s="170" t="s">
+        <v>42</v>
       </c>
       <c r="M22" s="35"/>
       <c r="N22" s="34"/>
       <c r="O22" s="28"/>
       <c r="P22" s="28"/>
-      <c r="Q22" s="214"/>
+      <c r="Q22" s="215"/>
     </row>
     <row r="23" ht="15.75" customHeight="1" spans="1:17">
       <c r="A23" s="28"/>
       <c r="B23" s="33"/>
       <c r="C23" s="40" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D23" s="40"/>
       <c r="E23" s="41"/>
       <c r="F23" s="41" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G23" s="42">
         <f>SUM(G21:G22)</f>
         <v>11</v>
       </c>
       <c r="H23" s="41" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I23" s="154"/>
       <c r="J23" s="35"/>
-      <c r="K23" s="170"/>
+      <c r="K23" s="171"/>
       <c r="L23" s="34"/>
       <c r="M23" s="34"/>
       <c r="N23" s="34"/>
       <c r="O23" s="28"/>
       <c r="P23" s="28"/>
-      <c r="Q23" s="214"/>
+      <c r="Q23" s="215"/>
     </row>
     <row r="24" ht="15.75" customHeight="1" spans="1:17">
       <c r="A24" s="1"/>
@@ -3111,42 +3119,42 @@
       <c r="N24" s="1"/>
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
-      <c r="Q24" s="214"/>
+      <c r="Q24" s="215"/>
     </row>
     <row r="25" ht="15.75" customHeight="1" spans="1:17">
       <c r="A25" s="1"/>
       <c r="B25" s="6"/>
       <c r="C25" s="46" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D25" s="46" t="s">
         <v>4</v>
       </c>
       <c r="E25" s="46" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F25" s="47" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G25" s="23"/>
       <c r="H25" s="48"/>
       <c r="I25" s="47" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="J25" s="23"/>
       <c r="K25" s="46" t="s">
-        <v>51</v>
-      </c>
-      <c r="L25" s="171" t="s">
         <v>52</v>
       </c>
-      <c r="M25" s="172" t="s">
+      <c r="L25" s="172" t="s">
         <v>53</v>
+      </c>
+      <c r="M25" s="173" t="s">
+        <v>54</v>
       </c>
       <c r="N25" s="14"/>
       <c r="O25" s="14"/>
       <c r="P25" s="15"/>
-      <c r="Q25" s="214"/>
+      <c r="Q25" s="215"/>
     </row>
     <row r="26" ht="15.75" customHeight="1" spans="1:17">
       <c r="A26" s="1"/>
@@ -3157,21 +3165,21 @@
       <c r="F26" s="50"/>
       <c r="G26" s="51"/>
       <c r="H26" s="52" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="I26" s="50"/>
       <c r="J26" s="51"/>
       <c r="K26" s="49"/>
-      <c r="L26" s="173"/>
-      <c r="M26" s="172" t="s">
-        <v>55</v>
+      <c r="L26" s="174"/>
+      <c r="M26" s="173" t="s">
+        <v>56</v>
       </c>
       <c r="N26" s="15"/>
-      <c r="O26" s="174" t="s">
-        <v>56</v>
+      <c r="O26" s="175" t="s">
+        <v>57</v>
       </c>
       <c r="P26" s="15"/>
-      <c r="Q26" s="214"/>
+      <c r="Q26" s="215"/>
     </row>
     <row r="27" ht="31.5" customHeight="1" spans="1:17">
       <c r="A27" s="1"/>
@@ -3180,35 +3188,35 @@
       <c r="D27" s="49"/>
       <c r="E27" s="49"/>
       <c r="F27" s="46" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G27" s="46" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H27" s="53" t="s">
-        <v>59</v>
-      </c>
-      <c r="I27" s="175" t="s">
         <v>60</v>
       </c>
-      <c r="J27" s="46" t="s">
+      <c r="I27" s="176" t="s">
         <v>61</v>
       </c>
-      <c r="K27" s="49"/>
-      <c r="L27" s="173"/>
-      <c r="M27" s="176" t="s">
+      <c r="J27" s="46" t="s">
         <v>62</v>
       </c>
-      <c r="N27" s="176" t="s">
+      <c r="K27" s="49"/>
+      <c r="L27" s="174"/>
+      <c r="M27" s="177" t="s">
         <v>63</v>
       </c>
-      <c r="O27" s="176" t="s">
+      <c r="N27" s="177" t="s">
         <v>64</v>
       </c>
-      <c r="P27" s="176" t="s">
-        <v>63</v>
+      <c r="O27" s="177" t="s">
+        <v>65</v>
       </c>
-      <c r="Q27" s="214"/>
+      <c r="P27" s="177" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q27" s="215"/>
     </row>
     <row r="28" ht="15.6" spans="1:17">
       <c r="A28" s="1"/>
@@ -3221,13 +3229,13 @@
       <c r="H28" s="57"/>
       <c r="I28" s="57"/>
       <c r="J28" s="57"/>
-      <c r="K28" s="177"/>
-      <c r="L28" s="178"/>
-      <c r="M28" s="179"/>
-      <c r="N28" s="179"/>
-      <c r="O28" s="179"/>
-      <c r="P28" s="179"/>
-      <c r="Q28" s="214"/>
+      <c r="K28" s="178"/>
+      <c r="L28" s="179"/>
+      <c r="M28" s="180"/>
+      <c r="N28" s="180"/>
+      <c r="O28" s="180"/>
+      <c r="P28" s="180"/>
+      <c r="Q28" s="215"/>
     </row>
     <row r="29" ht="15.75" customHeight="1" spans="1:24">
       <c r="A29" s="1"/>
@@ -3246,27 +3254,27 @@
       <c r="N29" s="28"/>
       <c r="O29" s="28"/>
       <c r="P29" s="2"/>
-      <c r="Q29" s="214"/>
-      <c r="R29" s="215"/>
-      <c r="S29" s="215"/>
-      <c r="T29" s="215"/>
-      <c r="U29" s="215"/>
-      <c r="V29" s="215"/>
-      <c r="W29" s="215"/>
-      <c r="X29" s="215"/>
+      <c r="Q29" s="215"/>
+      <c r="R29" s="216"/>
+      <c r="S29" s="216"/>
+      <c r="T29" s="216"/>
+      <c r="U29" s="216"/>
+      <c r="V29" s="216"/>
+      <c r="W29" s="216"/>
+      <c r="X29" s="216"/>
     </row>
     <row r="30" ht="15.75" customHeight="1" spans="1:24">
       <c r="A30" s="1"/>
       <c r="B30" s="59"/>
       <c r="C30" s="60" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D30" s="61"/>
       <c r="E30" s="62"/>
       <c r="F30" s="62"/>
       <c r="G30" s="62"/>
       <c r="H30" s="62"/>
-      <c r="I30" s="180"/>
+      <c r="I30" s="181"/>
       <c r="J30" s="62"/>
       <c r="K30" s="61"/>
       <c r="L30" s="61"/>
@@ -3274,14 +3282,14 @@
       <c r="N30" s="61"/>
       <c r="O30" s="61"/>
       <c r="P30" s="62"/>
-      <c r="Q30" s="216"/>
-      <c r="R30" s="215"/>
-      <c r="S30" s="215"/>
-      <c r="T30" s="215"/>
-      <c r="U30" s="215"/>
-      <c r="V30" s="215"/>
-      <c r="W30" s="215"/>
-      <c r="X30" s="215"/>
+      <c r="Q30" s="217"/>
+      <c r="R30" s="216"/>
+      <c r="S30" s="216"/>
+      <c r="T30" s="216"/>
+      <c r="U30" s="216"/>
+      <c r="V30" s="216"/>
+      <c r="W30" s="216"/>
+      <c r="X30" s="216"/>
     </row>
     <row r="31" ht="15.75" customHeight="1" spans="1:24">
       <c r="A31" s="1"/>
@@ -3293,44 +3301,44 @@
       <c r="G31" s="64"/>
       <c r="H31" s="64"/>
       <c r="I31" s="136"/>
-      <c r="J31" s="181"/>
-      <c r="K31" s="182"/>
-      <c r="L31" s="182"/>
-      <c r="M31" s="182"/>
-      <c r="N31" s="182"/>
-      <c r="O31" s="182"/>
-      <c r="P31" s="183"/>
-      <c r="Q31" s="214"/>
-      <c r="R31" s="215"/>
-      <c r="S31" s="215"/>
-      <c r="T31" s="215"/>
-      <c r="U31" s="215"/>
-      <c r="V31" s="215"/>
-      <c r="W31" s="215"/>
-      <c r="X31" s="215"/>
+      <c r="J31" s="182"/>
+      <c r="K31" s="183"/>
+      <c r="L31" s="183"/>
+      <c r="M31" s="183"/>
+      <c r="N31" s="183"/>
+      <c r="O31" s="183"/>
+      <c r="P31" s="184"/>
+      <c r="Q31" s="215"/>
+      <c r="R31" s="216"/>
+      <c r="S31" s="216"/>
+      <c r="T31" s="216"/>
+      <c r="U31" s="216"/>
+      <c r="V31" s="216"/>
+      <c r="W31" s="216"/>
+      <c r="X31" s="216"/>
     </row>
     <row r="32" ht="17.25" customHeight="1" spans="1:17">
       <c r="A32" s="1"/>
       <c r="B32" s="3"/>
       <c r="C32" s="65" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D32" s="66"/>
       <c r="E32" s="67" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F32" s="68"/>
       <c r="G32" s="68"/>
       <c r="H32" s="68"/>
-      <c r="I32" s="184"/>
-      <c r="J32" s="185"/>
-      <c r="K32" s="186"/>
-      <c r="L32" s="186"/>
-      <c r="M32" s="186"/>
-      <c r="N32" s="186"/>
-      <c r="O32" s="186"/>
-      <c r="P32" s="187"/>
-      <c r="Q32" s="213"/>
+      <c r="I32" s="185"/>
+      <c r="J32" s="186"/>
+      <c r="K32" s="187"/>
+      <c r="L32" s="187"/>
+      <c r="M32" s="187"/>
+      <c r="N32" s="187"/>
+      <c r="O32" s="187"/>
+      <c r="P32" s="188"/>
+      <c r="Q32" s="214"/>
     </row>
     <row r="33" ht="25.5" customHeight="1" spans="1:17">
       <c r="A33" s="1"/>
@@ -3338,97 +3346,97 @@
       <c r="C33" s="69"/>
       <c r="D33" s="70"/>
       <c r="E33" s="69" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F33" s="71"/>
       <c r="G33" s="69"/>
       <c r="H33" s="71"/>
-      <c r="I33" s="188"/>
-      <c r="J33" s="185"/>
-      <c r="K33" s="186"/>
-      <c r="L33" s="186"/>
-      <c r="M33" s="186"/>
-      <c r="N33" s="186"/>
-      <c r="O33" s="186"/>
-      <c r="P33" s="187"/>
-      <c r="Q33" s="214"/>
+      <c r="I33" s="189"/>
+      <c r="J33" s="186"/>
+      <c r="K33" s="187"/>
+      <c r="L33" s="187"/>
+      <c r="M33" s="187"/>
+      <c r="N33" s="187"/>
+      <c r="O33" s="187"/>
+      <c r="P33" s="188"/>
+      <c r="Q33" s="215"/>
     </row>
     <row r="34" ht="20.25" customHeight="1" spans="1:17">
       <c r="A34" s="1"/>
       <c r="B34" s="6"/>
       <c r="C34" s="72" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D34" s="73"/>
       <c r="E34" s="74" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F34" s="75"/>
       <c r="G34" s="75"/>
       <c r="H34" s="75"/>
-      <c r="I34" s="188"/>
-      <c r="J34" s="185"/>
-      <c r="K34" s="186"/>
-      <c r="L34" s="186"/>
-      <c r="M34" s="186"/>
-      <c r="N34" s="186"/>
-      <c r="O34" s="186"/>
-      <c r="P34" s="187"/>
-      <c r="Q34" s="214"/>
+      <c r="I34" s="189"/>
+      <c r="J34" s="186"/>
+      <c r="K34" s="187"/>
+      <c r="L34" s="187"/>
+      <c r="M34" s="187"/>
+      <c r="N34" s="187"/>
+      <c r="O34" s="187"/>
+      <c r="P34" s="188"/>
+      <c r="Q34" s="215"/>
     </row>
     <row r="35" ht="16.5" customHeight="1" spans="1:17">
       <c r="A35" s="1"/>
       <c r="B35" s="6"/>
       <c r="C35" s="76" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D35" s="77"/>
       <c r="E35" s="74" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F35" s="78"/>
       <c r="G35" s="74" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H35" s="78"/>
-      <c r="I35" s="188"/>
-      <c r="J35" s="185"/>
-      <c r="K35" s="186"/>
-      <c r="L35" s="186"/>
-      <c r="M35" s="186"/>
-      <c r="N35" s="186"/>
-      <c r="O35" s="186"/>
-      <c r="P35" s="187"/>
-      <c r="Q35" s="214"/>
+      <c r="I35" s="189"/>
+      <c r="J35" s="186"/>
+      <c r="K35" s="187"/>
+      <c r="L35" s="187"/>
+      <c r="M35" s="187"/>
+      <c r="N35" s="187"/>
+      <c r="O35" s="187"/>
+      <c r="P35" s="188"/>
+      <c r="Q35" s="215"/>
     </row>
     <row r="36" ht="15.75" customHeight="1" spans="1:17">
       <c r="A36" s="1"/>
       <c r="B36" s="6"/>
       <c r="C36" s="79" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D36" s="80"/>
       <c r="E36" s="81" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F36" s="82"/>
       <c r="G36" s="82"/>
       <c r="H36" s="83"/>
-      <c r="I36" s="188"/>
-      <c r="J36" s="185"/>
-      <c r="K36" s="186"/>
-      <c r="L36" s="186"/>
-      <c r="M36" s="186"/>
-      <c r="N36" s="186"/>
-      <c r="O36" s="186"/>
-      <c r="P36" s="187"/>
-      <c r="Q36" s="214"/>
+      <c r="I36" s="189"/>
+      <c r="J36" s="186"/>
+      <c r="K36" s="187"/>
+      <c r="L36" s="187"/>
+      <c r="M36" s="187"/>
+      <c r="N36" s="187"/>
+      <c r="O36" s="187"/>
+      <c r="P36" s="188"/>
+      <c r="Q36" s="215"/>
     </row>
     <row r="37" ht="15.75" customHeight="1" spans="1:17">
       <c r="A37" s="1"/>
       <c r="B37" s="6"/>
       <c r="C37" s="79" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D37" s="80"/>
       <c r="E37" s="84">
@@ -3436,47 +3444,47 @@
       </c>
       <c r="F37" s="85"/>
       <c r="G37" s="84" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H37" s="85"/>
-      <c r="I37" s="188"/>
-      <c r="J37" s="185"/>
-      <c r="K37" s="186"/>
-      <c r="L37" s="186"/>
-      <c r="M37" s="186"/>
-      <c r="N37" s="186"/>
-      <c r="O37" s="186"/>
-      <c r="P37" s="187"/>
-      <c r="Q37" s="214"/>
+      <c r="I37" s="189"/>
+      <c r="J37" s="186"/>
+      <c r="K37" s="187"/>
+      <c r="L37" s="187"/>
+      <c r="M37" s="187"/>
+      <c r="N37" s="187"/>
+      <c r="O37" s="187"/>
+      <c r="P37" s="188"/>
+      <c r="Q37" s="215"/>
     </row>
     <row r="38" ht="15.75" customHeight="1" spans="1:17">
       <c r="A38" s="1"/>
       <c r="B38" s="6"/>
       <c r="C38" s="79" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D38" s="80"/>
       <c r="E38" s="81" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F38" s="82"/>
       <c r="G38" s="82"/>
       <c r="H38" s="83"/>
-      <c r="I38" s="188"/>
-      <c r="J38" s="185"/>
-      <c r="K38" s="186"/>
-      <c r="L38" s="186"/>
-      <c r="M38" s="186"/>
-      <c r="N38" s="186"/>
-      <c r="O38" s="186"/>
-      <c r="P38" s="187"/>
-      <c r="Q38" s="214"/>
+      <c r="I38" s="189"/>
+      <c r="J38" s="186"/>
+      <c r="K38" s="187"/>
+      <c r="L38" s="187"/>
+      <c r="M38" s="187"/>
+      <c r="N38" s="187"/>
+      <c r="O38" s="187"/>
+      <c r="P38" s="188"/>
+      <c r="Q38" s="215"/>
     </row>
     <row r="39" ht="15.75" customHeight="1" spans="1:17">
       <c r="A39" s="1"/>
       <c r="B39" s="6"/>
       <c r="C39" s="79" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D39" s="80"/>
       <c r="E39" s="86">
@@ -3484,18 +3492,18 @@
       </c>
       <c r="F39" s="87"/>
       <c r="G39" s="88" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H39" s="89"/>
-      <c r="I39" s="188"/>
-      <c r="J39" s="185"/>
-      <c r="K39" s="186"/>
-      <c r="L39" s="186"/>
-      <c r="M39" s="186"/>
-      <c r="N39" s="186"/>
-      <c r="O39" s="186"/>
-      <c r="P39" s="187"/>
-      <c r="Q39" s="214"/>
+      <c r="I39" s="189"/>
+      <c r="J39" s="186"/>
+      <c r="K39" s="187"/>
+      <c r="L39" s="187"/>
+      <c r="M39" s="187"/>
+      <c r="N39" s="187"/>
+      <c r="O39" s="187"/>
+      <c r="P39" s="188"/>
+      <c r="Q39" s="215"/>
     </row>
     <row r="40" ht="15.75" customHeight="1" spans="1:17">
       <c r="A40" s="1"/>
@@ -3503,22 +3511,22 @@
       <c r="C40" s="76"/>
       <c r="D40" s="90"/>
       <c r="E40" s="88" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F40" s="89"/>
       <c r="G40" s="88" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H40" s="89"/>
-      <c r="I40" s="188"/>
-      <c r="J40" s="189"/>
-      <c r="K40" s="190"/>
-      <c r="L40" s="190"/>
-      <c r="M40" s="190"/>
-      <c r="N40" s="190"/>
-      <c r="O40" s="190"/>
-      <c r="P40" s="191"/>
-      <c r="Q40" s="214"/>
+      <c r="I40" s="189"/>
+      <c r="J40" s="190"/>
+      <c r="K40" s="191"/>
+      <c r="L40" s="191"/>
+      <c r="M40" s="191"/>
+      <c r="N40" s="191"/>
+      <c r="O40" s="191"/>
+      <c r="P40" s="192"/>
+      <c r="Q40" s="215"/>
     </row>
     <row r="41" ht="15.75" customHeight="1" spans="1:17">
       <c r="A41" s="1"/>
@@ -3529,36 +3537,36 @@
       <c r="F41" s="92"/>
       <c r="G41" s="92"/>
       <c r="H41" s="92"/>
-      <c r="I41" s="192"/>
+      <c r="I41" s="193"/>
       <c r="J41" s="91"/>
-      <c r="K41" s="193"/>
+      <c r="K41" s="194"/>
       <c r="L41" s="62"/>
-      <c r="M41" s="194"/>
-      <c r="N41" s="194"/>
+      <c r="M41" s="195"/>
+      <c r="N41" s="195"/>
       <c r="O41" s="133"/>
       <c r="P41" s="133"/>
-      <c r="Q41" s="214"/>
+      <c r="Q41" s="215"/>
     </row>
     <row r="42" ht="15.75" customHeight="1" spans="1:17">
       <c r="A42" s="1"/>
       <c r="B42" s="3"/>
       <c r="C42" s="30" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D42" s="93"/>
       <c r="E42" s="94"/>
       <c r="F42" s="94"/>
       <c r="G42" s="94"/>
       <c r="H42" s="94"/>
-      <c r="I42" s="195"/>
+      <c r="I42" s="196"/>
       <c r="J42" s="94"/>
-      <c r="K42" s="196"/>
+      <c r="K42" s="197"/>
       <c r="L42" s="93"/>
       <c r="M42" s="93"/>
       <c r="N42" s="93"/>
       <c r="O42" s="93"/>
       <c r="P42" s="93"/>
-      <c r="Q42" s="213"/>
+      <c r="Q42" s="214"/>
     </row>
     <row r="43" ht="15.75" customHeight="1" spans="1:17">
       <c r="A43" s="1"/>
@@ -3569,7 +3577,7 @@
       <c r="F43" s="43"/>
       <c r="G43" s="43"/>
       <c r="H43" s="43"/>
-      <c r="I43" s="197"/>
+      <c r="I43" s="198"/>
       <c r="J43" s="43"/>
       <c r="K43" s="44"/>
       <c r="L43" s="95"/>
@@ -3577,7 +3585,7 @@
       <c r="N43" s="95"/>
       <c r="O43" s="95"/>
       <c r="P43" s="95"/>
-      <c r="Q43" s="214"/>
+      <c r="Q43" s="215"/>
     </row>
     <row r="44" ht="15.75" customHeight="1" spans="1:17">
       <c r="A44" s="1"/>
@@ -3588,7 +3596,7 @@
       <c r="F44" s="43"/>
       <c r="G44" s="43"/>
       <c r="H44" s="43"/>
-      <c r="I44" s="197"/>
+      <c r="I44" s="198"/>
       <c r="J44" s="43"/>
       <c r="K44" s="44"/>
       <c r="L44" s="44"/>
@@ -3596,7 +3604,7 @@
       <c r="N44" s="44"/>
       <c r="O44" s="44"/>
       <c r="P44" s="44"/>
-      <c r="Q44" s="214"/>
+      <c r="Q44" s="215"/>
     </row>
     <row r="45" ht="15.75" customHeight="1" spans="1:17">
       <c r="A45" s="1"/>
@@ -3607,7 +3615,7 @@
       <c r="F45" s="97"/>
       <c r="G45" s="97"/>
       <c r="H45" s="97"/>
-      <c r="I45" s="198"/>
+      <c r="I45" s="199"/>
       <c r="J45" s="97"/>
       <c r="K45" s="96"/>
       <c r="L45" s="96"/>
@@ -3615,13 +3623,13 @@
       <c r="N45" s="96"/>
       <c r="O45" s="96"/>
       <c r="P45" s="96"/>
-      <c r="Q45" s="213"/>
+      <c r="Q45" s="214"/>
     </row>
     <row r="46" ht="15.75" customHeight="1" spans="1:17">
       <c r="A46" s="1"/>
       <c r="B46" s="6"/>
       <c r="C46" s="98" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D46" s="98"/>
       <c r="E46" s="98"/>
@@ -3636,7 +3644,7 @@
       <c r="N46" s="1"/>
       <c r="O46" s="1"/>
       <c r="P46" s="1"/>
-      <c r="Q46" s="214"/>
+      <c r="Q46" s="215"/>
     </row>
     <row r="47" ht="15.75" customHeight="1" spans="1:17">
       <c r="A47" s="1"/>
@@ -3655,53 +3663,53 @@
       <c r="N47" s="1"/>
       <c r="O47" s="1"/>
       <c r="P47" s="1"/>
-      <c r="Q47" s="214"/>
+      <c r="Q47" s="215"/>
     </row>
     <row r="48" ht="16.5" customHeight="1" spans="1:17">
       <c r="A48" s="1"/>
       <c r="B48" s="6"/>
       <c r="C48" s="101" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D48" s="102"/>
       <c r="E48" s="103"/>
       <c r="F48" s="54"/>
       <c r="G48" s="104" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H48" s="105"/>
-      <c r="I48" s="199"/>
+      <c r="I48" s="200"/>
       <c r="J48" s="54"/>
-      <c r="K48" s="200"/>
+      <c r="K48" s="201"/>
       <c r="L48" s="104" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="M48" s="105"/>
       <c r="N48" s="105"/>
       <c r="O48" s="105"/>
-      <c r="P48" s="199"/>
-      <c r="Q48" s="214"/>
+      <c r="P48" s="200"/>
+      <c r="Q48" s="215"/>
     </row>
     <row r="49" ht="15.75" customHeight="1" spans="1:17">
       <c r="A49" s="1"/>
       <c r="B49" s="6"/>
       <c r="C49" s="106" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D49" s="107"/>
       <c r="E49" s="108"/>
       <c r="F49" s="54"/>
       <c r="G49" s="109"/>
       <c r="H49" s="110"/>
-      <c r="I49" s="201"/>
+      <c r="I49" s="202"/>
       <c r="J49" s="54"/>
-      <c r="K49" s="200"/>
+      <c r="K49" s="201"/>
       <c r="L49" s="109"/>
       <c r="M49" s="110"/>
       <c r="N49" s="110"/>
       <c r="O49" s="110"/>
-      <c r="P49" s="201"/>
-      <c r="Q49" s="214"/>
+      <c r="P49" s="202"/>
+      <c r="Q49" s="215"/>
     </row>
     <row r="50" ht="15.75" customHeight="1" spans="1:17">
       <c r="A50" s="1"/>
@@ -3712,15 +3720,15 @@
       <c r="F50" s="54"/>
       <c r="G50" s="114"/>
       <c r="H50" s="115"/>
-      <c r="I50" s="202"/>
+      <c r="I50" s="203"/>
       <c r="J50" s="54"/>
-      <c r="K50" s="200"/>
-      <c r="L50" s="203"/>
-      <c r="M50" s="204"/>
-      <c r="N50" s="204"/>
-      <c r="O50" s="204"/>
+      <c r="K50" s="201"/>
+      <c r="L50" s="204"/>
+      <c r="M50" s="205"/>
+      <c r="N50" s="205"/>
+      <c r="O50" s="205"/>
       <c r="P50" s="113"/>
-      <c r="Q50" s="214"/>
+      <c r="Q50" s="215"/>
     </row>
     <row r="51" ht="15.75" customHeight="1" spans="1:17">
       <c r="A51" s="1"/>
@@ -3731,15 +3739,15 @@
       <c r="F51" s="54"/>
       <c r="G51" s="119"/>
       <c r="H51" s="100"/>
-      <c r="I51" s="205"/>
+      <c r="I51" s="206"/>
       <c r="J51" s="54"/>
-      <c r="K51" s="200"/>
-      <c r="L51" s="206"/>
+      <c r="K51" s="201"/>
+      <c r="L51" s="207"/>
       <c r="M51" s="54"/>
       <c r="N51" s="54"/>
       <c r="O51" s="54"/>
       <c r="P51" s="118"/>
-      <c r="Q51" s="214"/>
+      <c r="Q51" s="215"/>
     </row>
     <row r="52" ht="15.75" customHeight="1" spans="1:17">
       <c r="A52" s="1"/>
@@ -3750,15 +3758,15 @@
       <c r="F52" s="54"/>
       <c r="G52" s="119"/>
       <c r="H52" s="100"/>
-      <c r="I52" s="205"/>
+      <c r="I52" s="206"/>
       <c r="J52" s="54"/>
-      <c r="K52" s="200"/>
-      <c r="L52" s="206"/>
+      <c r="K52" s="201"/>
+      <c r="L52" s="207"/>
       <c r="M52" s="54"/>
       <c r="N52" s="54"/>
       <c r="O52" s="54"/>
       <c r="P52" s="118"/>
-      <c r="Q52" s="214"/>
+      <c r="Q52" s="215"/>
     </row>
     <row r="53" ht="15.75" customHeight="1" spans="1:17">
       <c r="A53" s="1"/>
@@ -3769,15 +3777,15 @@
       <c r="F53" s="54"/>
       <c r="G53" s="119"/>
       <c r="H53" s="100"/>
-      <c r="I53" s="205"/>
+      <c r="I53" s="206"/>
       <c r="J53" s="54"/>
-      <c r="K53" s="200"/>
-      <c r="L53" s="206"/>
+      <c r="K53" s="201"/>
+      <c r="L53" s="207"/>
       <c r="M53" s="54"/>
       <c r="N53" s="54"/>
       <c r="O53" s="54"/>
       <c r="P53" s="118"/>
-      <c r="Q53" s="214"/>
+      <c r="Q53" s="215"/>
     </row>
     <row r="54" ht="16.35" spans="1:17">
       <c r="A54" s="1"/>
@@ -3788,40 +3796,40 @@
       <c r="F54" s="54"/>
       <c r="G54" s="126"/>
       <c r="H54" s="127"/>
-      <c r="I54" s="207"/>
+      <c r="I54" s="208"/>
       <c r="J54" s="54"/>
-      <c r="K54" s="200"/>
-      <c r="L54" s="208"/>
-      <c r="M54" s="209"/>
-      <c r="N54" s="209"/>
-      <c r="O54" s="209"/>
-      <c r="P54" s="210"/>
-      <c r="Q54" s="214"/>
+      <c r="K54" s="201"/>
+      <c r="L54" s="209"/>
+      <c r="M54" s="210"/>
+      <c r="N54" s="210"/>
+      <c r="O54" s="210"/>
+      <c r="P54" s="211"/>
+      <c r="Q54" s="215"/>
     </row>
     <row r="55" ht="15.75" customHeight="1" spans="1:17">
       <c r="A55" s="1"/>
       <c r="B55" s="6"/>
       <c r="C55" s="128" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D55" s="129"/>
       <c r="E55" s="130"/>
       <c r="F55" s="54"/>
       <c r="G55" s="131" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H55" s="132"/>
-      <c r="I55" s="211"/>
+      <c r="I55" s="212"/>
       <c r="J55" s="54"/>
-      <c r="K55" s="200"/>
+      <c r="K55" s="201"/>
       <c r="L55" s="131" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="M55" s="132"/>
       <c r="N55" s="132"/>
       <c r="O55" s="132"/>
-      <c r="P55" s="211"/>
-      <c r="Q55" s="214"/>
+      <c r="P55" s="212"/>
+      <c r="Q55" s="215"/>
     </row>
     <row r="56" ht="15.75" customHeight="1" spans="1:17">
       <c r="A56" s="1"/>
@@ -3832,15 +3840,15 @@
       <c r="F56" s="62"/>
       <c r="G56" s="62"/>
       <c r="H56" s="62"/>
-      <c r="I56" s="180"/>
+      <c r="I56" s="181"/>
       <c r="J56" s="62"/>
-      <c r="K56" s="212"/>
+      <c r="K56" s="213"/>
       <c r="L56" s="133"/>
       <c r="M56" s="133"/>
       <c r="N56" s="133"/>
       <c r="O56" s="133"/>
       <c r="P56" s="133"/>
-      <c r="Q56" s="216"/>
+      <c r="Q56" s="217"/>
     </row>
     <row r="57" ht="15.75" customHeight="1" spans="1:16">
       <c r="A57" s="1"/>
@@ -3887,7 +3895,7 @@
       <c r="F59" s="43"/>
       <c r="G59" s="43"/>
       <c r="H59" s="43"/>
-      <c r="I59" s="197"/>
+      <c r="I59" s="198"/>
       <c r="J59" s="43"/>
       <c r="K59" s="135"/>
       <c r="L59" s="95"/>

</xml_diff>

<commit_message>
BAST: 1. Fix BAST template by removing the default value in excel file. 2. Fix the numbering of member data.
</commit_message>
<xml_diff>
--- a/bast/static/bast/BAST.xlsx
+++ b/bast/static/bast/BAST.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="81">
   <si>
     <t xml:space="preserve">BERITA ACARA SERAH TERIMA PUSAT GEMPA NASIONAL  </t>
   </si>
@@ -89,58 +89,28 @@
     <t>Semua Operator</t>
   </si>
   <si>
-    <t>Gian G.</t>
-  </si>
-  <si>
-    <t>Hadir</t>
-  </si>
-  <si>
     <t>JOPEN/Swift/TOAST</t>
-  </si>
-  <si>
-    <t>Jerisman</t>
   </si>
   <si>
     <t>Focal Mechanism/Qc</t>
   </si>
   <si>
-    <t>Hendra</t>
-  </si>
-  <si>
     <t>Disseminasi, RTSP</t>
-  </si>
-  <si>
-    <t>Valdo</t>
   </si>
   <si>
     <t>Tide Gauge, Buoy, GPS</t>
   </si>
   <si>
-    <t>Rosi</t>
-  </si>
-  <si>
     <t>Komunikasi Publik</t>
-  </si>
-  <si>
-    <t>Naufal</t>
   </si>
   <si>
     <t>Berita gempa, web, BAST</t>
   </si>
   <si>
-    <t>Fajar</t>
-  </si>
-  <si>
     <t>Laporan (1 jam-an)</t>
   </si>
   <si>
-    <t>Maryam</t>
-  </si>
-  <si>
     <t>Narasi &amp; Press Release</t>
-  </si>
-  <si>
-    <t>Trismahargyono</t>
   </si>
   <si>
     <t>Jumlah Petugas Yang Hadir</t>
@@ -2466,7 +2436,7 @@
   <dimension ref="A1:X976"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4259259259259" defaultRowHeight="15" customHeight="1"/>
@@ -2684,15 +2654,9 @@
       </c>
       <c r="H9" s="15"/>
       <c r="I9" s="157"/>
-      <c r="J9" s="158">
-        <v>1</v>
-      </c>
-      <c r="K9" s="159" t="s">
-        <v>20</v>
-      </c>
-      <c r="L9" s="160" t="s">
-        <v>21</v>
-      </c>
+      <c r="J9" s="158"/>
+      <c r="K9" s="159"/>
+      <c r="L9" s="160"/>
       <c r="M9" s="14"/>
       <c r="N9" s="14"/>
       <c r="O9" s="15"/>
@@ -2706,7 +2670,7 @@
         <v>2</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E10" s="14"/>
       <c r="F10" s="15"/>
@@ -2715,15 +2679,9 @@
       </c>
       <c r="H10" s="15"/>
       <c r="I10" s="157"/>
-      <c r="J10" s="158">
-        <v>2</v>
-      </c>
-      <c r="K10" s="161" t="s">
-        <v>23</v>
-      </c>
-      <c r="L10" s="160" t="s">
-        <v>21</v>
-      </c>
+      <c r="J10" s="158"/>
+      <c r="K10" s="161"/>
+      <c r="L10" s="160"/>
       <c r="M10" s="14"/>
       <c r="N10" s="14"/>
       <c r="O10" s="15"/>
@@ -2737,7 +2695,7 @@
         <v>3</v>
       </c>
       <c r="D11" s="18" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E11" s="14"/>
       <c r="F11" s="15"/>
@@ -2746,15 +2704,9 @@
       </c>
       <c r="H11" s="15"/>
       <c r="I11" s="157"/>
-      <c r="J11" s="158">
-        <v>3</v>
-      </c>
-      <c r="K11" s="161" t="s">
-        <v>25</v>
-      </c>
-      <c r="L11" s="160" t="s">
-        <v>21</v>
-      </c>
+      <c r="J11" s="158"/>
+      <c r="K11" s="161"/>
+      <c r="L11" s="160"/>
       <c r="M11" s="14"/>
       <c r="N11" s="14"/>
       <c r="O11" s="15"/>
@@ -2768,7 +2720,7 @@
         <v>4</v>
       </c>
       <c r="D12" s="18" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E12" s="14"/>
       <c r="F12" s="15"/>
@@ -2777,15 +2729,9 @@
       </c>
       <c r="H12" s="15"/>
       <c r="I12" s="157"/>
-      <c r="J12" s="158">
-        <v>4</v>
-      </c>
-      <c r="K12" s="161" t="s">
-        <v>27</v>
-      </c>
-      <c r="L12" s="160" t="s">
-        <v>21</v>
-      </c>
+      <c r="J12" s="158"/>
+      <c r="K12" s="161"/>
+      <c r="L12" s="160"/>
       <c r="M12" s="14"/>
       <c r="N12" s="14"/>
       <c r="O12" s="15"/>
@@ -2799,7 +2745,7 @@
         <v>5</v>
       </c>
       <c r="D13" s="18" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="E13" s="14"/>
       <c r="F13" s="15"/>
@@ -2808,15 +2754,9 @@
       </c>
       <c r="H13" s="15"/>
       <c r="I13" s="157"/>
-      <c r="J13" s="158">
-        <v>5</v>
-      </c>
-      <c r="K13" s="161" t="s">
-        <v>29</v>
-      </c>
-      <c r="L13" s="160" t="s">
-        <v>21</v>
-      </c>
+      <c r="J13" s="158"/>
+      <c r="K13" s="161"/>
+      <c r="L13" s="160"/>
       <c r="M13" s="14"/>
       <c r="N13" s="14"/>
       <c r="O13" s="15"/>
@@ -2830,7 +2770,7 @@
         <v>6</v>
       </c>
       <c r="D14" s="18" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="E14" s="14"/>
       <c r="F14" s="15"/>
@@ -2839,15 +2779,9 @@
       </c>
       <c r="H14" s="15"/>
       <c r="I14" s="157"/>
-      <c r="J14" s="158">
-        <v>6</v>
-      </c>
-      <c r="K14" s="161" t="s">
-        <v>31</v>
-      </c>
-      <c r="L14" s="160" t="s">
-        <v>21</v>
-      </c>
+      <c r="J14" s="158"/>
+      <c r="K14" s="161"/>
+      <c r="L14" s="160"/>
       <c r="M14" s="14"/>
       <c r="N14" s="14"/>
       <c r="O14" s="15"/>
@@ -2861,7 +2795,7 @@
         <v>7</v>
       </c>
       <c r="D15" s="18" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="E15" s="14"/>
       <c r="F15" s="15"/>
@@ -2870,15 +2804,9 @@
       </c>
       <c r="H15" s="15"/>
       <c r="I15" s="134"/>
-      <c r="J15" s="158">
-        <v>7</v>
-      </c>
-      <c r="K15" s="161" t="s">
-        <v>33</v>
-      </c>
-      <c r="L15" s="160" t="s">
-        <v>21</v>
-      </c>
+      <c r="J15" s="158"/>
+      <c r="K15" s="161"/>
+      <c r="L15" s="160"/>
       <c r="M15" s="14"/>
       <c r="N15" s="14"/>
       <c r="O15" s="15"/>
@@ -2892,7 +2820,7 @@
         <v>8</v>
       </c>
       <c r="D16" s="18" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="E16" s="14"/>
       <c r="F16" s="15"/>
@@ -2901,15 +2829,9 @@
       </c>
       <c r="H16" s="15"/>
       <c r="I16" s="157"/>
-      <c r="J16" s="158">
-        <v>8</v>
-      </c>
-      <c r="K16" s="162" t="s">
-        <v>35</v>
-      </c>
-      <c r="L16" s="160" t="s">
-        <v>21</v>
-      </c>
+      <c r="J16" s="158"/>
+      <c r="K16" s="162"/>
+      <c r="L16" s="160"/>
       <c r="M16" s="14"/>
       <c r="N16" s="14"/>
       <c r="O16" s="15"/>
@@ -2923,7 +2845,7 @@
         <v>9</v>
       </c>
       <c r="D17" s="21" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="E17" s="22"/>
       <c r="F17" s="23"/>
@@ -2932,15 +2854,9 @@
       </c>
       <c r="H17" s="23"/>
       <c r="I17" s="157"/>
-      <c r="J17" s="158">
-        <v>9</v>
-      </c>
-      <c r="K17" s="161" t="s">
-        <v>37</v>
-      </c>
-      <c r="L17" s="160" t="s">
-        <v>21</v>
-      </c>
+      <c r="J17" s="158"/>
+      <c r="K17" s="161"/>
+      <c r="L17" s="160"/>
       <c r="M17" s="14"/>
       <c r="N17" s="14"/>
       <c r="O17" s="15"/>
@@ -2958,21 +2874,19 @@
       <c r="H18" s="22"/>
       <c r="I18" s="134"/>
       <c r="J18" s="163" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="K18" s="51"/>
-      <c r="L18" s="164">
-        <v>9</v>
-      </c>
+      <c r="L18" s="164"/>
       <c r="M18" s="165" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="N18" s="165"/>
       <c r="O18" s="166"/>
       <c r="P18" s="1"/>
       <c r="Q18" s="215"/>
     </row>
-    <row r="19" spans="1:17">
+    <row r="19" ht="15.15" spans="1:17">
       <c r="A19" s="1"/>
       <c r="B19" s="6"/>
       <c r="C19" s="2"/>
@@ -2995,7 +2909,7 @@
       <c r="A20" s="28"/>
       <c r="B20" s="29"/>
       <c r="C20" s="30" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D20" s="31"/>
       <c r="E20" s="32"/>
@@ -3016,26 +2930,26 @@
       <c r="A21" s="28"/>
       <c r="B21" s="33"/>
       <c r="C21" s="34" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="D21" s="34"/>
       <c r="E21" s="35"/>
       <c r="F21" s="35" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="G21" s="36">
         <v>7</v>
       </c>
       <c r="H21" s="35" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="I21" s="154"/>
       <c r="J21" s="170" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="K21" s="170"/>
       <c r="L21" s="170" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="M21" s="35"/>
       <c r="N21" s="34"/>
@@ -3047,26 +2961,26 @@
       <c r="A22" s="28"/>
       <c r="B22" s="33"/>
       <c r="C22" s="37" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="D22" s="37"/>
       <c r="E22" s="38"/>
       <c r="F22" s="38" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="G22" s="39">
         <v>4</v>
       </c>
       <c r="H22" s="38" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="I22" s="154"/>
       <c r="J22" s="218" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="K22" s="170"/>
       <c r="L22" s="170" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="M22" s="35"/>
       <c r="N22" s="34"/>
@@ -3078,19 +2992,19 @@
       <c r="A23" s="28"/>
       <c r="B23" s="33"/>
       <c r="C23" s="40" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="D23" s="40"/>
       <c r="E23" s="41"/>
       <c r="F23" s="41" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="G23" s="42">
         <f>SUM(G21:G22)</f>
         <v>11</v>
       </c>
       <c r="H23" s="41" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="I23" s="154"/>
       <c r="J23" s="35"/>
@@ -3125,31 +3039,31 @@
       <c r="A25" s="1"/>
       <c r="B25" s="6"/>
       <c r="C25" s="46" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="D25" s="46" t="s">
         <v>4</v>
       </c>
       <c r="E25" s="46" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="F25" s="47" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="G25" s="23"/>
       <c r="H25" s="48"/>
       <c r="I25" s="47" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="J25" s="23"/>
       <c r="K25" s="46" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="L25" s="172" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="M25" s="173" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="N25" s="14"/>
       <c r="O25" s="14"/>
@@ -3165,18 +3079,18 @@
       <c r="F26" s="50"/>
       <c r="G26" s="51"/>
       <c r="H26" s="52" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="I26" s="50"/>
       <c r="J26" s="51"/>
       <c r="K26" s="49"/>
       <c r="L26" s="174"/>
       <c r="M26" s="173" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="N26" s="15"/>
       <c r="O26" s="175" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="P26" s="15"/>
       <c r="Q26" s="215"/>
@@ -3188,33 +3102,33 @@
       <c r="D27" s="49"/>
       <c r="E27" s="49"/>
       <c r="F27" s="46" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="G27" s="46" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="H27" s="53" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="I27" s="176" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="J27" s="46" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="K27" s="49"/>
       <c r="L27" s="174"/>
       <c r="M27" s="177" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="N27" s="177" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="O27" s="177" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="P27" s="177" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="Q27" s="215"/>
     </row>
@@ -3267,7 +3181,7 @@
       <c r="A30" s="1"/>
       <c r="B30" s="59"/>
       <c r="C30" s="60" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="D30" s="61"/>
       <c r="E30" s="62"/>
@@ -3321,11 +3235,11 @@
       <c r="A32" s="1"/>
       <c r="B32" s="3"/>
       <c r="C32" s="65" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="D32" s="66"/>
       <c r="E32" s="67" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="F32" s="68"/>
       <c r="G32" s="68"/>
@@ -3346,7 +3260,7 @@
       <c r="C33" s="69"/>
       <c r="D33" s="70"/>
       <c r="E33" s="69" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="F33" s="71"/>
       <c r="G33" s="69"/>
@@ -3365,11 +3279,11 @@
       <c r="A34" s="1"/>
       <c r="B34" s="6"/>
       <c r="C34" s="72" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="D34" s="73"/>
       <c r="E34" s="74" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="F34" s="75"/>
       <c r="G34" s="75"/>
@@ -3388,15 +3302,15 @@
       <c r="A35" s="1"/>
       <c r="B35" s="6"/>
       <c r="C35" s="76" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="D35" s="77"/>
       <c r="E35" s="74" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="F35" s="78"/>
       <c r="G35" s="74" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="H35" s="78"/>
       <c r="I35" s="189"/>
@@ -3413,11 +3327,11 @@
       <c r="A36" s="1"/>
       <c r="B36" s="6"/>
       <c r="C36" s="79" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="D36" s="80"/>
       <c r="E36" s="81" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="F36" s="82"/>
       <c r="G36" s="82"/>
@@ -3436,7 +3350,7 @@
       <c r="A37" s="1"/>
       <c r="B37" s="6"/>
       <c r="C37" s="79" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="D37" s="80"/>
       <c r="E37" s="84">
@@ -3444,7 +3358,7 @@
       </c>
       <c r="F37" s="85"/>
       <c r="G37" s="84" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="H37" s="85"/>
       <c r="I37" s="189"/>
@@ -3461,11 +3375,11 @@
       <c r="A38" s="1"/>
       <c r="B38" s="6"/>
       <c r="C38" s="79" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="D38" s="80"/>
       <c r="E38" s="81" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="F38" s="82"/>
       <c r="G38" s="82"/>
@@ -3484,7 +3398,7 @@
       <c r="A39" s="1"/>
       <c r="B39" s="6"/>
       <c r="C39" s="79" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="D39" s="80"/>
       <c r="E39" s="86">
@@ -3492,7 +3406,7 @@
       </c>
       <c r="F39" s="87"/>
       <c r="G39" s="88" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="H39" s="89"/>
       <c r="I39" s="189"/>
@@ -3511,11 +3425,11 @@
       <c r="C40" s="76"/>
       <c r="D40" s="90"/>
       <c r="E40" s="88" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="F40" s="89"/>
       <c r="G40" s="88" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="H40" s="89"/>
       <c r="I40" s="189"/>
@@ -3551,7 +3465,7 @@
       <c r="A42" s="1"/>
       <c r="B42" s="3"/>
       <c r="C42" s="30" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="D42" s="93"/>
       <c r="E42" s="94"/>
@@ -3629,7 +3543,7 @@
       <c r="A46" s="1"/>
       <c r="B46" s="6"/>
       <c r="C46" s="98" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="D46" s="98"/>
       <c r="E46" s="98"/>
@@ -3669,20 +3583,20 @@
       <c r="A48" s="1"/>
       <c r="B48" s="6"/>
       <c r="C48" s="101" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="D48" s="102"/>
       <c r="E48" s="103"/>
       <c r="F48" s="54"/>
       <c r="G48" s="104" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="H48" s="105"/>
       <c r="I48" s="200"/>
       <c r="J48" s="54"/>
       <c r="K48" s="201"/>
       <c r="L48" s="104" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="M48" s="105"/>
       <c r="N48" s="105"/>
@@ -3694,7 +3608,7 @@
       <c r="A49" s="1"/>
       <c r="B49" s="6"/>
       <c r="C49" s="106" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="D49" s="107"/>
       <c r="E49" s="108"/>
@@ -3810,20 +3724,20 @@
       <c r="A55" s="1"/>
       <c r="B55" s="6"/>
       <c r="C55" s="128" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="D55" s="129"/>
       <c r="E55" s="130"/>
       <c r="F55" s="54"/>
       <c r="G55" s="131" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="H55" s="132"/>
       <c r="I55" s="212"/>
       <c r="J55" s="54"/>
       <c r="K55" s="201"/>
       <c r="L55" s="131" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="M55" s="132"/>
       <c r="N55" s="132"/>

</xml_diff>